<commit_message>
Included mezz calculations + summary
</commit_message>
<xml_diff>
--- a/borrower_cf.xlsx
+++ b/borrower_cf.xlsx
@@ -829,13 +829,13 @@
         <v>40851063.82978723</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>14317259.53416658</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>-14317259.53416658</v>
       </c>
       <c r="G7" t="n">
         <v>132324265.8621302</v>
@@ -859,7 +859,7 @@
         <v>2042553.191489362</v>
       </c>
       <c r="N7" t="n">
-        <v>-0</v>
+        <v>-14317259.53416658</v>
       </c>
       <c r="O7" t="n">
         <v>-3268085.106382979</v>
@@ -868,10 +868,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q7" t="n">
-        <v>-5943884.102098872</v>
+        <v>-20261143.63626546</v>
       </c>
       <c r="R7" t="n">
-        <v>-33787648.04947903</v>
+        <v>-48104907.58364561</v>
       </c>
     </row>
     <row r="8">
@@ -887,13 +887,13 @@
         <v>47021276.59574468</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>29818032.94573001</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>-15500773.41156343</v>
       </c>
       <c r="G8" t="n">
         <v>170793672.1428188</v>
@@ -917,7 +917,7 @@
         <v>2351063.829787234</v>
       </c>
       <c r="N8" t="n">
-        <v>-0</v>
+        <v>-15500773.41156343</v>
       </c>
       <c r="O8" t="n">
         <v>-3761702.127659575</v>
@@ -926,10 +926,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q8" t="n">
-        <v>-6043054.747758931</v>
+        <v>-21543828.15932235</v>
       </c>
       <c r="R8" t="n">
-        <v>-39830702.79723796</v>
+        <v>-69648735.74296796</v>
       </c>
     </row>
     <row r="9">
@@ -945,13 +945,13 @@
         <v>53191489.36170213</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>45761494.75871766</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>-15943461.81298766</v>
       </c>
       <c r="G9" t="n">
         <v>213354687.4478233</v>
@@ -975,7 +975,7 @@
         <v>2659574.468085106</v>
       </c>
       <c r="N9" t="n">
-        <v>-0</v>
+        <v>-15943461.81298766</v>
       </c>
       <c r="O9" t="n">
         <v>-4255319.14893617</v>
@@ -984,10 +984,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q9" t="n">
-        <v>-6131295.2660685</v>
+        <v>-22074757.07905615</v>
       </c>
       <c r="R9" t="n">
-        <v>-45961998.06330647</v>
+        <v>-91723492.82202412</v>
       </c>
     </row>
     <row r="10">
@@ -1003,13 +1003,13 @@
         <v>59361702.12765957</v>
       </c>
       <c r="D10" t="n">
-        <v>6661770.509111762</v>
+        <v>60661770.50911177</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-6661770.509111762</v>
+        <v>-14900275.75039411</v>
       </c>
       <c r="G10" t="n">
         <v>259769292.9031703</v>
@@ -1033,7 +1033,7 @@
         <v>2968085.106382979</v>
       </c>
       <c r="N10" t="n">
-        <v>-6661770.509111762</v>
+        <v>-14900275.75039411</v>
       </c>
       <c r="O10" t="n">
         <v>-4748936.170212766</v>
@@ -1042,10 +1042,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q10" t="n">
-        <v>-12870455.34358143</v>
+        <v>-21108960.58486378</v>
       </c>
       <c r="R10" t="n">
-        <v>-58832453.4068879</v>
+        <v>-112832453.4068879</v>
       </c>
     </row>
     <row r="11">
@@ -1061,7 +1061,7 @@
         <v>65531914.89361702</v>
       </c>
       <c r="D11" t="n">
-        <v>6661770.509111762</v>
+        <v>60661770.50911177</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1103,7 +1103,7 @@
         <v>-6275302.630404534</v>
       </c>
       <c r="R11" t="n">
-        <v>-65107756.03729244</v>
+        <v>-119107756.0372924</v>
       </c>
     </row>
     <row r="12">
@@ -1119,7 +1119,7 @@
         <v>71702127.65957446</v>
       </c>
       <c r="D12" t="n">
-        <v>14539984.33019322</v>
+        <v>68539984.33019322</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         <v>3585106.382978723</v>
       </c>
       <c r="N12" t="n">
-        <v>-7878213.82108146</v>
+        <v>-7878213.821081452</v>
       </c>
       <c r="O12" t="n">
         <v>-5736170.212765957</v>
@@ -1158,10 +1158,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q12" t="n">
-        <v>-14209441.65239664</v>
+        <v>-14209441.65239663</v>
       </c>
       <c r="R12" t="n">
-        <v>-79317197.68968907</v>
+        <v>-133317197.6896891</v>
       </c>
     </row>
     <row r="13">
@@ -1177,7 +1177,7 @@
         <v>77872340.42553191</v>
       </c>
       <c r="D13" t="n">
-        <v>22522795.20482963</v>
+        <v>76522795.20482963</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>-14359350.4892801</v>
       </c>
       <c r="R13" t="n">
-        <v>-93676548.17896917</v>
+        <v>-147676548.1789692</v>
       </c>
     </row>
     <row r="14">
@@ -1235,7 +1235,7 @@
         <v>84042553.19148937</v>
       </c>
       <c r="D14" t="n">
-        <v>29934451.55832386</v>
+        <v>83934451.55832386</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>-13822973.51132639</v>
       </c>
       <c r="R14" t="n">
-        <v>-107499521.6902956</v>
+        <v>-161499521.6902956</v>
       </c>
     </row>
     <row r="15">
@@ -1293,7 +1293,7 @@
         <v>90212765.95744681</v>
       </c>
       <c r="D15" t="n">
-        <v>37531813.19470388</v>
+        <v>91531813.19470388</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>-14033001.27470269</v>
       </c>
       <c r="R15" t="n">
-        <v>-121532522.9649983</v>
+        <v>-175532522.9649983</v>
       </c>
     </row>
     <row r="16">
@@ -1351,7 +1351,7 @@
         <v>96382978.72340426</v>
       </c>
       <c r="D16" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>-13253587.5065028</v>
       </c>
       <c r="R16" t="n">
-        <v>-134786110.4715011</v>
+        <v>-188786110.4715011</v>
       </c>
     </row>
     <row r="17">
@@ -1409,7 +1409,7 @@
         <v>102553191.4893617</v>
       </c>
       <c r="D17" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>-6453236.120978216</v>
       </c>
       <c r="R17" t="n">
-        <v>-141239346.5924793</v>
+        <v>-195239346.5924793</v>
       </c>
     </row>
     <row r="18">
@@ -1467,7 +1467,7 @@
         <v>108723404.2553191</v>
       </c>
       <c r="D18" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1509,7 +1509,7 @@
         <v>-6446668.478027413</v>
       </c>
       <c r="R18" t="n">
-        <v>-147686015.0705067</v>
+        <v>-201686015.0705067</v>
       </c>
     </row>
     <row r="19">
@@ -1525,7 +1525,7 @@
         <v>114893617.0212766</v>
       </c>
       <c r="D19" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         <v>-6429962.482147016</v>
       </c>
       <c r="R19" t="n">
-        <v>-154115977.5526537</v>
+        <v>-208115977.5526537</v>
       </c>
     </row>
     <row r="20">
@@ -1583,7 +1583,7 @@
         <v>121063829.787234</v>
       </c>
       <c r="D20" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1625,7 +1625,7 @@
         <v>-6403197.310779111</v>
       </c>
       <c r="R20" t="n">
-        <v>-160519174.8634328</v>
+        <v>-214519174.8634328</v>
       </c>
     </row>
     <row r="21">
@@ -1641,7 +1641,7 @@
         <v>127234042.5531915</v>
       </c>
       <c r="D21" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>-6366452.141365796</v>
       </c>
       <c r="R21" t="n">
-        <v>-166885627.0047986</v>
+        <v>-220885627.0047986</v>
       </c>
     </row>
     <row r="22">
@@ -1699,7 +1699,7 @@
         <v>133404255.3191489</v>
       </c>
       <c r="D22" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1741,7 +1741,7 @@
         <v>-6319806.151349148</v>
       </c>
       <c r="R22" t="n">
-        <v>-173205433.1561477</v>
+        <v>-227205433.1561478</v>
       </c>
     </row>
     <row r="23">
@@ -1757,7 +1757,7 @@
         <v>139574468.0851064</v>
       </c>
       <c r="D23" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>-6263338.518171262</v>
       </c>
       <c r="R23" t="n">
-        <v>-179468771.674319</v>
+        <v>-233468771.674319</v>
       </c>
     </row>
     <row r="24">
@@ -1815,7 +1815,7 @@
         <v>145744680.8510638</v>
       </c>
       <c r="D24" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1857,7 +1857,7 @@
         <v>-6197128.419274233</v>
       </c>
       <c r="R24" t="n">
-        <v>-185665900.0935932</v>
+        <v>-239665900.0935933</v>
       </c>
     </row>
     <row r="25">
@@ -1873,7 +1873,7 @@
         <v>144779689.5353063</v>
       </c>
       <c r="D25" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1915,7 +1915,7 @@
         <v>-5920536.209309159</v>
       </c>
       <c r="R25" t="n">
-        <v>-191586436.3029024</v>
+        <v>-245586436.3029024</v>
       </c>
     </row>
     <row r="26">
@@ -1931,7 +1931,7 @@
         <v>107324991.9445118</v>
       </c>
       <c r="D26" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E26" t="n">
         <v>6566936.019001676</v>
@@ -1973,7 +1973,7 @@
         <v>-4636734.416985562</v>
       </c>
       <c r="R26" t="n">
-        <v>-196223170.719888</v>
+        <v>-250223170.719888</v>
       </c>
     </row>
     <row r="27">
@@ -1989,7 +1989,7 @@
         <v>106251742.0250666</v>
       </c>
       <c r="D27" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E27" t="n">
         <v>19516146.48659175</v>
@@ -2031,7 +2031,7 @@
         <v>-4446326.644362995</v>
       </c>
       <c r="R27" t="n">
-        <v>-200669497.364251</v>
+        <v>-254669497.364251</v>
       </c>
     </row>
     <row r="28">
@@ -2047,7 +2047,7 @@
         <v>105189224.604816</v>
       </c>
       <c r="D28" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E28" t="n">
         <v>38419839.39864769</v>
@@ -2089,7 +2089,7 @@
         <v>-4269337.597997583</v>
       </c>
       <c r="R28" t="n">
-        <v>-204938834.9622485</v>
+        <v>-258938834.9622486</v>
       </c>
     </row>
     <row r="29">
@@ -2105,7 +2105,7 @@
         <v>104137332.3587677</v>
       </c>
       <c r="D29" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E29" t="n">
         <v>63287830.54850446</v>
@@ -2147,7 +2147,7 @@
         <v>-4092639.984134545</v>
       </c>
       <c r="R29" t="n">
-        <v>-209031474.9463831</v>
+        <v>-263031474.9463831</v>
       </c>
     </row>
     <row r="30">
@@ -2163,7 +2163,7 @@
         <v>103095959.0351801</v>
       </c>
       <c r="D30" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E30" t="n">
         <v>93685509.97845159</v>
@@ -2205,7 +2205,7 @@
         <v>-3929524.010079514</v>
       </c>
       <c r="R30" t="n">
-        <v>-212960998.9564626</v>
+        <v>-266960998.9564626</v>
       </c>
     </row>
     <row r="31">
@@ -2221,7 +2221,7 @@
         <v>102064999.4448283</v>
       </c>
       <c r="D31" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E31" t="n">
         <v>129707368.763854</v>
@@ -2263,7 +2263,7 @@
         <v>-3764125.874430548</v>
       </c>
       <c r="R31" t="n">
-        <v>-216725124.8308931</v>
+        <v>-270725124.8308932</v>
       </c>
     </row>
     <row r="32">
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -2321,7 +2321,7 @@
         <v>-808729.7071339241</v>
       </c>
       <c r="R32" t="n">
-        <v>-217533854.538027</v>
+        <v>-271533854.5380271</v>
       </c>
     </row>
     <row r="33">
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -2379,7 +2379,7 @@
         <v>-924313.3919224991</v>
       </c>
       <c r="R33" t="n">
-        <v>-218458167.9299496</v>
+        <v>-272458167.9299496</v>
       </c>
     </row>
     <row r="34">
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2437,7 +2437,7 @@
         <v>-1048847.768009327</v>
       </c>
       <c r="R34" t="n">
-        <v>-219507015.6979589</v>
+        <v>-273507015.6979589</v>
       </c>
     </row>
     <row r="35">
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2495,7 +2495,7 @@
         <v>-1182253.657952322</v>
       </c>
       <c r="R35" t="n">
-        <v>-220689269.3559112</v>
+        <v>-274689269.3559112</v>
       </c>
     </row>
     <row r="36">
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -2553,7 +2553,7 @@
         <v>-1324451.884309394</v>
       </c>
       <c r="R36" t="n">
-        <v>-222013721.2402206</v>
+        <v>-276013721.2402206</v>
       </c>
     </row>
     <row r="37">
@@ -2569,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>44335814.46764934</v>
+        <v>98335814.46764934</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -2611,7 +2611,7 @@
         <v>-1475363.269638453</v>
       </c>
       <c r="R37" t="n">
-        <v>-223489084.509859</v>
+        <v>-277489084.5098591</v>
       </c>
     </row>
     <row r="38">
@@ -2627,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>44335814.46764934</v>
+        <v>44816535.90076101</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>-0</v>
+        <v>53519278.56688833</v>
       </c>
       <c r="O38" t="n">
         <v>-0</v>
@@ -2666,10 +2666,10 @@
         <v>-5000000</v>
       </c>
       <c r="Q38" t="n">
-        <v>-1634908.636497411</v>
+        <v>51884369.93039092</v>
       </c>
       <c r="R38" t="n">
-        <v>-225123993.1463564</v>
+        <v>-225604714.5794682</v>
       </c>
     </row>
     <row r="39">
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>44108415.10408677</v>
+        <v>61951990.08296807</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>44335814.46764934</v>
+        <v>44816535.90076101</v>
       </c>
       <c r="O39" t="n">
         <v>-0</v>
@@ -2724,7 +2724,7 @@
         <v>-5000000</v>
       </c>
       <c r="Q39" t="n">
-        <v>42532805.66020516</v>
+        <v>43013527.09331683</v>
       </c>
       <c r="R39" t="n">
         <v>-182591187.4861513</v>
@@ -2746,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>145262929.5440292</v>
+        <v>163164919.7441755</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -2804,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>240562670.9487408</v>
+        <v>258523267.6063859</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>-2164556.85183278</v>
       </c>
       <c r="R41" t="n">
-        <v>-186735328.9430207</v>
+        <v>-186735328.9430208</v>
       </c>
     </row>
     <row r="42">
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>329710322.3033209</v>
+        <v>347729717.2807562</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -2920,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>412410241.1426102</v>
+        <v>430488626.9302343</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -2959,7 +2959,7 @@
         <v>-2559373.983267548</v>
       </c>
       <c r="R43" t="n">
-        <v>-191652549.2966787</v>
+        <v>-191652549.2966788</v>
       </c>
     </row>
     <row r="44">
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>488368465.033231</v>
+        <v>506506034.7516059</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -3017,7 +3017,7 @@
         <v>-2769060.51302202</v>
       </c>
       <c r="R44" t="n">
-        <v>-194421609.8097007</v>
+        <v>-194421609.8097008</v>
       </c>
     </row>
     <row r="45">
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>557292717.0735738</v>
+        <v>575489664.4754883</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -3075,7 +3075,7 @@
         <v>-2986826.782211766</v>
       </c>
       <c r="R45" t="n">
-        <v>-197408436.5919125</v>
+        <v>-197408436.5919126</v>
       </c>
     </row>
     <row r="46">
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>618892411.4117904</v>
+        <v>637148930.8843291</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -3133,7 +3133,7 @@
         <v>-3212593.613394694</v>
       </c>
       <c r="R46" t="n">
-        <v>-200621030.2053072</v>
+        <v>-200621030.2053073</v>
       </c>
     </row>
     <row r="47">
@@ -3152,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>672878658.7818497</v>
+        <v>691194945.3484702</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -3191,7 +3191,7 @@
         <v>-3446281.829128718</v>
       </c>
       <c r="R47" t="n">
-        <v>-204067312.0344359</v>
+        <v>-204067312.034436</v>
       </c>
     </row>
     <row r="48">
@@ -3210,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>718964272.0577195</v>
+        <v>737340521.3803352</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>

</xml_diff>